<commit_message>
Out Of Office and Reset Password
</commit_message>
<xml_diff>
--- a/ExcelDataProvider/DataSheets.xlsx
+++ b/ExcelDataProvider/DataSheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -279,43 +279,43 @@
     <t>admin</t>
   </si>
   <si>
+    <t>Bourbon Offshore Asia Pte Ltd</t>
+  </si>
+  <si>
+    <t>Contract Holder Name</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>axel.hartmann78@yopmail.com</t>
+  </si>
+  <si>
+    <t>Vallianz Offshore marine Pte Ltd</t>
+  </si>
+  <si>
+    <t>Viddacom (VD)</t>
+  </si>
+  <si>
+    <t>LDT KB</t>
+  </si>
+  <si>
+    <t>Ardella  (ardella4@yopmail.com)</t>
+  </si>
+  <si>
+    <t>BELAIT SHIPPING COMPANY (B) SDN BHD</t>
+  </si>
+  <si>
+    <t>OMBAK BIRU SATU</t>
+  </si>
+  <si>
+    <t>NOBLE VIKING</t>
+  </si>
+  <si>
+    <t>OVID</t>
+  </si>
+  <si>
     <t>123qwe</t>
-  </si>
-  <si>
-    <t>Bourbon Offshore Asia Pte Ltd</t>
-  </si>
-  <si>
-    <t>Contract Holder Name</t>
-  </si>
-  <si>
-    <t>AUS</t>
-  </si>
-  <si>
-    <t>axel.hartmann78@yopmail.com</t>
-  </si>
-  <si>
-    <t>Vallianz Offshore marine Pte Ltd</t>
-  </si>
-  <si>
-    <t>Viddacom (VD)</t>
-  </si>
-  <si>
-    <t>LDT KB</t>
-  </si>
-  <si>
-    <t>Ardella  (ardella4@yopmail.com)</t>
-  </si>
-  <si>
-    <t>BELAIT SHIPPING COMPANY (B) SDN BHD</t>
-  </si>
-  <si>
-    <t>OMBAK BIRU SATU</t>
-  </si>
-  <si>
-    <t>NOBLE VIKING</t>
-  </si>
-  <si>
-    <t>OVID</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -684,7 +684,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -781,10 +781,10 @@
         <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -799,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -844,22 +844,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
         <v>91</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>87</v>
       </c>
-      <c r="D2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" t="s">
-        <v>88</v>
-      </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2">
         <v>2026</v>
@@ -948,7 +948,7 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2">
         <v>7856458</v>
@@ -1091,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1111,13 +1111,13 @@
         <v>2021</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
         <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>